<commit_message>
Start working on task 3
</commit_message>
<xml_diff>
--- a/lab4/plots.xlsx
+++ b/lab4/plots.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>n</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>log(n)</t>
+  </si>
+  <si>
+    <t>Ratio with previous</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1074,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1281,7 +1283,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1403,7 +1404,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1478,7 +1478,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8006,15 +8005,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="D1" sqref="D1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8024,8 +8023,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -8037,7 +8039,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -8048,8 +8050,12 @@
       <c r="C3">
         <v>1E-4</v>
       </c>
+      <c r="D3">
+        <f>C2/C3</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4000</v>
       </c>
@@ -8060,8 +8066,12 @@
       <c r="C4">
         <v>1E-4</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D8" si="1">C3/C4</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -8072,8 +8082,12 @@
       <c r="C5">
         <v>0.1</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16000</v>
       </c>
@@ -8084,8 +8098,12 @@
       <c r="C6">
         <v>0.2</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>32000</v>
       </c>
@@ -8095,6 +8113,10 @@
       </c>
       <c r="C7">
         <v>0.5</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -8107,15 +8129,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8125,8 +8147,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -8138,7 +8163,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -8149,8 +8174,12 @@
       <c r="C3">
         <v>1E-4</v>
       </c>
+      <c r="D3">
+        <f>C2/C3</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4000</v>
       </c>
@@ -8161,8 +8190,12 @@
       <c r="C4">
         <v>1E-4</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="1">C3/C4</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -8173,8 +8206,12 @@
       <c r="C5">
         <v>1E-4</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16000</v>
       </c>
@@ -8185,8 +8222,12 @@
       <c r="C6">
         <v>1E-4</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>32000</v>
       </c>
@@ -8196,6 +8237,10 @@
       </c>
       <c r="C7">
         <v>1E-4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8208,15 +8253,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="D1" sqref="D1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8226,8 +8271,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -8239,7 +8287,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -8250,8 +8298,12 @@
       <c r="C3">
         <v>1.7</v>
       </c>
+      <c r="D3">
+        <f>C2/C3</f>
+        <v>0.11764705882352942</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4000</v>
       </c>
@@ -8262,8 +8314,12 @@
       <c r="C4">
         <v>13.5</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="1">C3/C4</f>
+        <v>0.12592592592592591</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -8274,8 +8330,12 @@
       <c r="C5">
         <v>85.7</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.15752625437572929</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16000</v>
       </c>
@@ -8286,8 +8346,12 @@
       <c r="C6">
         <v>676.4</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.12670017740981668</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>32000</v>
       </c>
@@ -8297,6 +8361,10 @@
       </c>
       <c r="C7">
         <v>5471.1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.12363144523039242</v>
       </c>
     </row>
   </sheetData>
@@ -8309,15 +8377,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8327,8 +8395,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -8340,7 +8411,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -8351,8 +8422,12 @@
       <c r="C3">
         <v>0.1</v>
       </c>
+      <c r="D3">
+        <f>C2/C3</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4000</v>
       </c>
@@ -8363,8 +8438,12 @@
       <c r="C4">
         <v>0.3</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="1">C3/C4</f>
+        <v>0.33333333333333337</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -8375,8 +8454,12 @@
       <c r="C5">
         <v>0.9</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16000</v>
       </c>
@@ -8387,8 +8470,12 @@
       <c r="C6">
         <v>3.7</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.24324324324324323</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>32000</v>
       </c>
@@ -8398,6 +8485,10 @@
       </c>
       <c r="C7">
         <v>15</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.24666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>